<commit_message>
Modelo entidad - relación y relacional de base de datos.
Se crea en equipo el modelo relacional de la base de datos y entidad
relacion.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2C7C8B-901A-449F-A5B3-A42A4242826A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCC907E-2790-45FA-B15C-D8E6E07638DF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,12 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -447,6 +441,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +758,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,84 +833,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="L4" s="20"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="15"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="15"/>
+      <c r="R4" s="20"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="15"/>
+      <c r="U4" s="20"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="14" t="s">
+      <c r="W4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="15"/>
+      <c r="X4" s="20"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="15"/>
+      <c r="AA4" s="20"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="14" t="s">
+      <c r="AC4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="15"/>
+      <c r="AD4" s="20"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="14" t="s">
+      <c r="AF4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="15"/>
+      <c r="AG4" s="20"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="14" t="s">
+      <c r="AI4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="15"/>
+      <c r="AJ4" s="20"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="14" t="s">
+      <c r="AL4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="15"/>
+      <c r="AM4" s="20"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="14" t="s">
+      <c r="AO4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="15"/>
+      <c r="AP4" s="20"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="14" t="s">
+      <c r="AR4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="15"/>
+      <c r="AS4" s="20"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="14" t="s">
+      <c r="AU4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="15"/>
+      <c r="AV4" s="20"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="14" t="s">
+      <c r="AX4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="14" t="s">
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="15"/>
+      <c r="BA4" s="20"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1050,109 +1050,113 @@
       <c r="D6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3</v>
+      </c>
       <c r="I6" s="8">
         <f>G6-H6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L17" si="0">I6-K6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O17" si="1">L6-N6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R17" si="2">O6-Q6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U17" si="3">R6-T6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X17" si="4">U6-W6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA17" si="5">X6-Z6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD17" si="6">AA6-AC6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG17" si="7">AD6-AF6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ17" si="8">AG6-AI6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM17" si="9">AJ6-AL6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP17" si="10">AM6-AO6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS17" si="11">AP6-AR6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV17" si="12">AS6-AU6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY17" si="13">AV6-AX6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA17" si="15">G6-AZ6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1161,14 +1165,18 @@
       <c r="D7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" ref="I7:I17" si="16">G7-H7</f>
         <v>0</v>
@@ -1259,7 +1267,7 @@
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
@@ -1272,7 +1280,7 @@
       <c r="D8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1383,7 +1391,7 @@
       <c r="D9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1496,7 +1504,7 @@
       <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1607,7 +1615,7 @@
       <c r="D11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1720,7 +1728,7 @@
       <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1831,7 +1839,7 @@
       <c r="D13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1942,7 +1950,7 @@
       <c r="D14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="18" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2053,7 +2061,7 @@
       <c r="D15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2164,7 +2172,7 @@
       <c r="D16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
         <v>41</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -2275,7 +2283,7 @@
       <c r="D17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -2388,7 +2396,7 @@
       <c r="D18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="18" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -2499,7 +2507,7 @@
       <c r="D19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -2607,10 +2615,10 @@
     <row r="20" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="5" t="s">

</xml_diff>

<commit_message>
Mapeo de base de datos, entidades y controladores.
Se mapea la base de datos en conjunto a entidades y controladores
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AD79E2-1B2B-4E20-9D93-20C4157223E0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -225,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,8 +451,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -751,14 +778,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,8 +1428,12 @@
       <c r="F9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
       <c r="I9" s="8">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -1493,7 +1524,7 @@
       </c>
       <c r="AZ9" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
@@ -2729,11 +2760,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2745,6 +2771,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2762,7 +2793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Segunda parte de implementacion del modulo administrar sesiones
Se implementa la segunda parte del modulo de administrar sesiones, aun
no esta terminada,tiene la funcionalidad de busqueda de usuarios y
validación de la sesion
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1138CCC-53C7-4242-ABE8-5A09BEB13155}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -225,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,7 +471,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -779,14 +773,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q15" sqref="Q15"/>
+      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,84 +1797,86 @@
         <v>3</v>
       </c>
       <c r="P12" s="10"/>
-      <c r="Q12" s="8"/>
+      <c r="Q12" s="8">
+        <v>2</v>
+      </c>
       <c r="R12" s="8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AZ12" s="11">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BA12" s="11">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2783,6 +2779,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2794,11 +2795,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2816,7 +2812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Modulo de catálogos terminado
Terminado con los faltantes de métodos correspondientes a otros módulos
y carga/guardado de imágenes de usuario. Se actualiza el modelo de
dominio, se agrega el campo "direccion" a la tabla Cliente (se modifica
el archivo Ared.sql), se actualizan modelo relacional y entidad, y se
actualizan plantillas de casos de uso y de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60D0C15-6257-4896-97DD-D1D19D692AE4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -219,7 +225,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,7 +477,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -530,7 +536,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -563,9 +569,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,6 +621,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -773,14 +813,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,78 +1964,80 @@
         <v>-1</v>
       </c>
       <c r="S13" s="10"/>
-      <c r="T13" s="8"/>
+      <c r="T13" s="8">
+        <v>2</v>
+      </c>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.25">
@@ -2779,11 +2821,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2795,6 +2832,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2812,7 +2854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Modulo de sesiones terminado
Se implementa el modulo de sesiones, pantallas principales de ambos usuarios y edicion de usuario.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60D0C15-6257-4896-97DD-D1D19D692AE4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -225,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,7 +476,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -813,14 +812,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,78 +1844,80 @@
         <v>1</v>
       </c>
       <c r="S12" s="10"/>
-      <c r="T12" s="8"/>
+      <c r="T12" s="8">
+        <v>5</v>
+      </c>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="AZ12" s="11">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="BA12" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2821,6 +2822,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2832,11 +2838,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2854,7 +2855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Correcciones en los CU CRU gasto promocional y CRU egresos
Se implementa consultar gasto promocionl y consultar egresos, actualizaciones de las plantillas
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFE605-8F23-4E5C-A312-472FF5624B81}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -228,7 +227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,7 +479,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -816,14 +815,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z16" sqref="Z16"/>
+      <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,60 +2105,62 @@
         <v>2</v>
       </c>
       <c r="AB14" s="10"/>
-      <c r="AC14" s="8"/>
+      <c r="AC14" s="8">
+        <v>5</v>
+      </c>
       <c r="AD14" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AE14" s="10"/>
       <c r="AF14" s="8"/>
       <c r="AG14" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="AZ14" s="11">
         <f t="shared" si="14"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="BA14" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="15" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2840,11 +2841,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2856,6 +2852,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2873,7 +2874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Plantilla de iteracion correcta hasta el dia  3 de abril
corrección de plantilla hasta 3 de abril
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE7AABC-FB97-4766-A097-AB2645B0019F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
     <sheet name="Instructivo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$BB$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$BB$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>Columna</t>
   </si>
@@ -205,21 +199,6 @@
   </si>
   <si>
     <t>Modulo de pagos (parcial)</t>
-  </si>
-  <si>
-    <t>Modulo de grupos (parcial) :: modulo de catálogos (completo)</t>
-  </si>
-  <si>
-    <t>Reportes</t>
-  </si>
-  <si>
-    <t>Realizar documento de plan de pruebas</t>
-  </si>
-  <si>
-    <t>Realizar diagrama de paquetes</t>
-  </si>
-  <si>
-    <t>Realizar reporte de entrega</t>
   </si>
   <si>
     <t>Hecho</t>
@@ -228,7 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -384,24 +363,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -432,16 +398,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -480,7 +442,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -539,7 +501,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,26 +534,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,23 +569,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -816,14 +744,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BA20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:BA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="O9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="6" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI20" sqref="AI20"/>
+      <selection pane="bottomRight" activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,84 +826,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="20"/>
+      <c r="L4" s="18"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="20"/>
+      <c r="O4" s="18"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="20"/>
+      <c r="R4" s="18"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="20"/>
+      <c r="U4" s="18"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="19" t="s">
+      <c r="W4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="20"/>
+      <c r="X4" s="18"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="19" t="s">
+      <c r="Z4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="20"/>
+      <c r="AA4" s="18"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="19" t="s">
+      <c r="AC4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="20"/>
+      <c r="AD4" s="18"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="19" t="s">
+      <c r="AF4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="20"/>
+      <c r="AG4" s="18"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="19" t="s">
+      <c r="AI4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="20"/>
+      <c r="AJ4" s="18"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="19" t="s">
+      <c r="AL4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="20"/>
+      <c r="AM4" s="18"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="19" t="s">
+      <c r="AO4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="20"/>
+      <c r="AP4" s="18"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="19" t="s">
+      <c r="AR4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="20"/>
+      <c r="AS4" s="18"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="19" t="s">
+      <c r="AU4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="20"/>
+      <c r="AV4" s="18"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="19" t="s">
+      <c r="AX4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="20"/>
-      <c r="AZ4" s="19" t="s">
+      <c r="AY4" s="18"/>
+      <c r="AZ4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="20"/>
+      <c r="BA4" s="18"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1115,11 +1043,11 @@
       <c r="D6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G6" s="5">
         <v>2</v>
@@ -1134,93 +1062,93 @@
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
-        <f t="shared" ref="L6:L17" si="0">I6-K6</f>
+        <f t="shared" ref="L6:L15" si="0">I6-K6</f>
         <v>-1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
-        <f t="shared" ref="O6:O17" si="1">L6-N6</f>
+        <f t="shared" ref="O6:O15" si="1">L6-N6</f>
         <v>-1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
-        <f t="shared" ref="R6:R17" si="2">O6-Q6</f>
+        <f t="shared" ref="R6:R15" si="2">O6-Q6</f>
         <v>-1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
-        <f t="shared" ref="U6:U17" si="3">R6-T6</f>
+        <f t="shared" ref="U6:U15" si="3">R6-T6</f>
         <v>-1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
-        <f t="shared" ref="X6:X17" si="4">U6-W6</f>
+        <f t="shared" ref="X6:X15" si="4">U6-W6</f>
         <v>-1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
-        <f t="shared" ref="AA6:AA17" si="5">X6-Z6</f>
+        <f t="shared" ref="AA6:AA15" si="5">X6-Z6</f>
         <v>-1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
-        <f t="shared" ref="AD6:AD17" si="6">AA6-AC6</f>
+        <f t="shared" ref="AD6:AD15" si="6">AA6-AC6</f>
         <v>-1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
-        <f t="shared" ref="AG6:AG17" si="7">AD6-AF6</f>
+        <f t="shared" ref="AG6:AG15" si="7">AD6-AF6</f>
         <v>-1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
-        <f t="shared" ref="AJ6:AJ17" si="8">AG6-AI6</f>
+        <f t="shared" ref="AJ6:AJ15" si="8">AG6-AI6</f>
         <v>-1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
-        <f t="shared" ref="AM6:AM17" si="9">AJ6-AL6</f>
+        <f t="shared" ref="AM6:AM15" si="9">AJ6-AL6</f>
         <v>-1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
-        <f t="shared" ref="AP6:AP17" si="10">AM6-AO6</f>
+        <f t="shared" ref="AP6:AP15" si="10">AM6-AO6</f>
         <v>-1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
-        <f t="shared" ref="AS6:AS17" si="11">AP6-AR6</f>
+        <f t="shared" ref="AS6:AS15" si="11">AP6-AR6</f>
         <v>-1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
-        <f t="shared" ref="AV6:AV17" si="12">AS6-AU6</f>
+        <f t="shared" ref="AV6:AV15" si="12">AS6-AU6</f>
         <v>-1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
-        <f t="shared" ref="AY6:AY17" si="13">AV6-AX6</f>
+        <f t="shared" ref="AY6:AY15" si="13">AV6-AX6</f>
         <v>-1</v>
       </c>
       <c r="AZ6" s="11">
-        <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
+        <f t="shared" ref="AZ6:AZ15" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
         <v>3</v>
       </c>
       <c r="BA6" s="11">
-        <f t="shared" ref="BA6:BA17" si="15">G6-AZ6</f>
+        <f t="shared" ref="BA6:BA15" si="15">G6-AZ6</f>
         <v>-1</v>
       </c>
     </row>
@@ -1230,11 +1158,11 @@
       <c r="D7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
@@ -1243,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="8">
-        <f t="shared" ref="I7:I17" si="16">G7-H7</f>
+        <f t="shared" ref="I7:I15" si="16">G7-H7</f>
         <v>0</v>
       </c>
       <c r="J7" s="10"/>
@@ -1345,11 +1273,11 @@
       <c r="D8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1460,11 +1388,11 @@
       <c r="D9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
@@ -1577,11 +1505,11 @@
       <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -1692,11 +1620,11 @@
       <c r="D11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1809,11 +1737,11 @@
       <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G12" s="5">
         <v>8</v>
@@ -1930,11 +1858,11 @@
       <c r="D13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G13" s="5">
         <v>8</v>
@@ -2051,7 +1979,7 @@
       <c r="D14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2114,54 +2042,56 @@
         <v>-3</v>
       </c>
       <c r="AE14" s="10"/>
-      <c r="AF14" s="8"/>
+      <c r="AF14" s="8">
+        <v>5</v>
+      </c>
       <c r="AG14" s="8">
         <f t="shared" si="7"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8">
         <f t="shared" si="8"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f t="shared" si="9"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f t="shared" si="10"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f t="shared" si="11"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f t="shared" si="13"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="AZ14" s="11">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="BA14" s="11">
         <f t="shared" si="15"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="15" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2170,7 +2100,7 @@
       <c r="D15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2283,574 +2213,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:53" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V16" s="10"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="8">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AK16" s="10"/>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AN16" s="10"/>
-      <c r="AO16" s="8"/>
-      <c r="AP16" s="8">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="10"/>
-      <c r="AR16" s="8"/>
-      <c r="AS16" s="8">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AT16" s="10"/>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AW16" s="10"/>
-      <c r="AX16" s="8"/>
-      <c r="AY16" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AZ16" s="11">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="BA16" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S17" s="10"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V17" s="10"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="8"/>
-      <c r="AG17" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="8"/>
-      <c r="AJ17" s="8">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="8"/>
-      <c r="AM17" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AN17" s="10"/>
-      <c r="AO17" s="8"/>
-      <c r="AP17" s="8">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="10"/>
-      <c r="AR17" s="8"/>
-      <c r="AS17" s="8">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AT17" s="10"/>
-      <c r="AU17" s="8"/>
-      <c r="AV17" s="8">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AW17" s="10"/>
-      <c r="AX17" s="8"/>
-      <c r="AY17" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AZ17" s="11">
-        <f>H17+K17+N17+Q17+T17+W17+Z17+AC17+AF17+AI17+AL17+AO17+AR17+AU17+AX17</f>
-        <v>0</v>
-      </c>
-      <c r="BA17" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8">
-        <f t="shared" ref="I18:I20" si="17">G18-H18</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8">
-        <f t="shared" ref="L18:L20" si="18">I18-K18</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8">
-        <f t="shared" ref="O18:O20" si="19">L18-N18</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8">
-        <f t="shared" ref="R18:R20" si="20">O18-Q18</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="10"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8">
-        <f t="shared" ref="U18:U20" si="21">R18-T18</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="10"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8">
-        <f t="shared" ref="X18:X20" si="22">U18-W18</f>
-        <v>0</v>
-      </c>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8">
-        <f t="shared" ref="AA18:AA20" si="23">X18-Z18</f>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="8">
-        <f t="shared" ref="AD18:AD20" si="24">AA18-AC18</f>
-        <v>0</v>
-      </c>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="8"/>
-      <c r="AG18" s="8">
-        <f t="shared" ref="AG18:AG20" si="25">AD18-AF18</f>
-        <v>0</v>
-      </c>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="8"/>
-      <c r="AJ18" s="8">
-        <f t="shared" ref="AJ18:AJ20" si="26">AG18-AI18</f>
-        <v>0</v>
-      </c>
-      <c r="AK18" s="10"/>
-      <c r="AL18" s="8"/>
-      <c r="AM18" s="8">
-        <f t="shared" ref="AM18:AM20" si="27">AJ18-AL18</f>
-        <v>0</v>
-      </c>
-      <c r="AN18" s="10"/>
-      <c r="AO18" s="8"/>
-      <c r="AP18" s="8">
-        <f t="shared" ref="AP18:AP20" si="28">AM18-AO18</f>
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="10"/>
-      <c r="AR18" s="8"/>
-      <c r="AS18" s="8">
-        <f t="shared" ref="AS18:AS20" si="29">AP18-AR18</f>
-        <v>0</v>
-      </c>
-      <c r="AT18" s="10"/>
-      <c r="AU18" s="8"/>
-      <c r="AV18" s="8">
-        <f t="shared" ref="AV18:AV20" si="30">AS18-AU18</f>
-        <v>0</v>
-      </c>
-      <c r="AW18" s="10"/>
-      <c r="AX18" s="8"/>
-      <c r="AY18" s="8">
-        <f t="shared" ref="AY18:AY20" si="31">AV18-AX18</f>
-        <v>0</v>
-      </c>
-      <c r="AZ18" s="11">
-        <f>H18+K18+N18+Q18+T18+W18+Z18+AC18+AF18+AI18+AL18+AO18+AR18+AU18+AX18</f>
-        <v>0</v>
-      </c>
-      <c r="BA18" s="11">
-        <f t="shared" ref="BA18:BA20" si="32">G18-AZ18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8">
-        <f t="shared" ref="I19" si="33">G19-H19</f>
-        <v>1</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8">
-        <f t="shared" ref="L19" si="34">I19-K19</f>
-        <v>1</v>
-      </c>
-      <c r="M19" s="10"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8">
-        <f t="shared" ref="O19" si="35">L19-N19</f>
-        <v>1</v>
-      </c>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8">
-        <f t="shared" ref="R19" si="36">O19-Q19</f>
-        <v>1</v>
-      </c>
-      <c r="S19" s="10"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8">
-        <f t="shared" ref="U19" si="37">R19-T19</f>
-        <v>1</v>
-      </c>
-      <c r="V19" s="10"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8">
-        <f t="shared" ref="X19" si="38">U19-W19</f>
-        <v>1</v>
-      </c>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8">
-        <f t="shared" ref="AA19" si="39">X19-Z19</f>
-        <v>1</v>
-      </c>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="8"/>
-      <c r="AD19" s="8">
-        <f t="shared" ref="AD19" si="40">AA19-AC19</f>
-        <v>1</v>
-      </c>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="8"/>
-      <c r="AG19" s="8">
-        <f t="shared" ref="AG19" si="41">AD19-AF19</f>
-        <v>1</v>
-      </c>
-      <c r="AH19" s="10"/>
-      <c r="AI19" s="8"/>
-      <c r="AJ19" s="8">
-        <f t="shared" ref="AJ19" si="42">AG19-AI19</f>
-        <v>1</v>
-      </c>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AM19" s="8">
-        <f t="shared" ref="AM19" si="43">AJ19-AL19</f>
-        <v>0</v>
-      </c>
-      <c r="AN19" s="10"/>
-      <c r="AO19" s="8"/>
-      <c r="AP19" s="8">
-        <f t="shared" ref="AP19" si="44">AM19-AO19</f>
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="10"/>
-      <c r="AR19" s="8"/>
-      <c r="AS19" s="8">
-        <f t="shared" ref="AS19" si="45">AP19-AR19</f>
-        <v>0</v>
-      </c>
-      <c r="AT19" s="10"/>
-      <c r="AU19" s="8"/>
-      <c r="AV19" s="8">
-        <f t="shared" ref="AV19" si="46">AS19-AU19</f>
-        <v>0</v>
-      </c>
-      <c r="AW19" s="10"/>
-      <c r="AX19" s="8"/>
-      <c r="AY19" s="8">
-        <f t="shared" ref="AY19" si="47">AV19-AX19</f>
-        <v>0</v>
-      </c>
-      <c r="AZ19" s="11">
-        <f>H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19</f>
-        <v>1</v>
-      </c>
-      <c r="BA19" s="11">
-        <f t="shared" ref="BA19" si="48">G19-AZ19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S20" s="10"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="V20" s="10"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="8">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="10"/>
-      <c r="AC20" s="8"/>
-      <c r="AD20" s="8">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="8"/>
-      <c r="AG20" s="8">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="AH20" s="10"/>
-      <c r="AI20" s="8"/>
-      <c r="AJ20" s="8">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="8"/>
-      <c r="AM20" s="8">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="AN20" s="10"/>
-      <c r="AO20" s="8"/>
-      <c r="AP20" s="8">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="10"/>
-      <c r="AR20" s="8"/>
-      <c r="AS20" s="8">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="AT20" s="10"/>
-      <c r="AU20" s="8"/>
-      <c r="AV20" s="8">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="AW20" s="10"/>
-      <c r="AX20" s="8"/>
-      <c r="AY20" s="8">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="AZ20" s="11" t="e">
-        <f>H20+K20+N20+Q20+T20+W20+Z20+AC20+AF20+AI20+AL20+AO20+AR20+AU20+AX20+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA20" s="11" t="e">
-        <f t="shared" si="32"/>
-        <v>#REF!</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2862,6 +2226,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2879,7 +2248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Correción de tareas realizadas
Se cambia de 'por iniciar' a 'hecho' en las ultimas 2 actividades de la
plantilla de lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 3ra Iteración.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C67CAC-274D-4606-A406-11F4B2623BDD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Columna</t>
   </si>
@@ -151,9 +157,6 @@
   </si>
   <si>
     <t>Mario</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>Base de datos</t>
@@ -207,7 +210,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,7 +445,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -501,7 +504,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,9 +537,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -569,6 +589,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -744,14 +781,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA15"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF14" sqref="AF14"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1074,17 @@
     </row>
     <row r="6" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="5">
         <v>2</v>
@@ -1156,13 +1193,13 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
@@ -1271,13 +1308,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1386,13 +1423,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
@@ -1499,17 +1536,17 @@
     </row>
     <row r="10" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -1618,13 +1655,13 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1731,17 +1768,17 @@
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="5">
         <v>8</v>
@@ -1856,13 +1893,13 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="5">
         <v>8</v>
@@ -1977,13 +2014,13 @@
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G14" s="5">
         <v>10</v>
@@ -2098,13 +2135,13 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G15" s="5">
         <v>6</v>
@@ -2215,6 +2252,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2226,11 +2268,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2248,7 +2285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>